<commit_message>
test cases 14, 15, and 16
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data1.xlsx
+++ b/com.espn/src/test/resources/test_data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.espn/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA77DAC5-847A-7041-B6C5-6DDE7A4F230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111624DA-426F-AC44-839E-D18642D302CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="9" activeTab="15" xr2:uid="{7B928831-F53C-A542-9271-10D2139B6158}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="9" activeTab="16" xr2:uid="{7B928831-F53C-A542-9271-10D2139B6158}"/>
   </bookViews>
   <sheets>
     <sheet name="PacificTeams" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="UnfollowButtonText" sheetId="11" r:id="rId14"/>
     <sheet name="NHLScoresText" sheetId="12" r:id="rId15"/>
     <sheet name="ESPNAccount" sheetId="20" r:id="rId16"/>
+    <sheet name="Editions" sheetId="21" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Golden State Warriors</t>
   </si>
@@ -156,6 +157,24 @@
   </si>
   <si>
     <t>Adil!</t>
+  </si>
+  <si>
+    <t>Edición: México</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Editie: Nederland</t>
+  </si>
+  <si>
+    <t>Edition: Australia</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -211,13 +230,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -776,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FB462D-78DF-014D-8E09-CAC36DE14C1D}">
   <dimension ref="A2:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -814,6 +834,50 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D441E4A-1F51-7944-A3C3-D895186D4928}">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3CA0B6-B515-1B48-9718-97BB94EB8CB8}">
   <dimension ref="A2"/>

</xml_diff>

<commit_message>
all 16 test cases passed
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/test_data1.xlsx
+++ b/com.espn/src/test/resources/test_data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.espn/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111624DA-426F-AC44-839E-D18642D302CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A68481B-8F5D-F348-B4C3-4582906B8179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="9" activeTab="16" xr2:uid="{7B928831-F53C-A542-9271-10D2139B6158}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="8" activeTab="14" xr2:uid="{7B928831-F53C-A542-9271-10D2139B6158}"/>
   </bookViews>
   <sheets>
     <sheet name="PacificTeams" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="RomanReignsTitleHistory" sheetId="9" r:id="rId9"/>
     <sheet name="LebronJamesStats" sheetId="10" r:id="rId10"/>
     <sheet name="IslamMakhachev" sheetId="4" r:id="rId11"/>
-    <sheet name="MMAP4P#1" sheetId="19" r:id="rId12"/>
+    <sheet name="MMAP4P" sheetId="19" r:id="rId12"/>
     <sheet name="AmericanLeagueEastTeams" sheetId="2" r:id="rId13"/>
     <sheet name="UnfollowButtonText" sheetId="11" r:id="rId14"/>
     <sheet name="NHLScoresText" sheetId="12" r:id="rId15"/>
@@ -99,9 +99,6 @@
     <t>2015|2</t>
   </si>
   <si>
-    <t>Saturday, November 5, 2022</t>
-  </si>
-  <si>
     <t>expected</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>FIFA World Cup Schedule</t>
   </si>
   <si>
-    <t>UFC featherweight champion</t>
-  </si>
-  <si>
     <t>adilkhaleque429@gmail.com</t>
   </si>
   <si>
@@ -175,6 +169,12 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>MMA pound-for-pound rankings</t>
+  </si>
+  <si>
+    <t>NHL Scoreboard</t>
   </si>
 </sst>
 </file>
@@ -567,10 +567,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -586,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -594,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -602,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -610,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +641,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -673,7 +673,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -686,17 +686,17 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +760,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562A714E-46DA-A445-A7D1-203BE3A34F7E}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,7 +784,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -811,19 +811,19 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -838,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D441E4A-1F51-7944-A3C3-D895186D4928}">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
@@ -851,26 +851,26 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1018,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +1042,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1066,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>